<commit_message>
feat: add codes and notes
</commit_message>
<xml_diff>
--- a/Udemy - Curso de Python 3 do básico ao avançado - com projetos reais/Secao_6_(04)/Aula_13_openpyxl/workbook.xlsx
+++ b/Udemy - Curso de Python 3 do básico ao avançado - com projetos reais/Secao_6_(04)/Aula_13_openpyxl/workbook.xlsx
@@ -1,65 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Nome</t>
-  </si>
-  <si>
-    <t>Idade</t>
-  </si>
-  <si>
-    <t>Nota</t>
-  </si>
-  <si>
-    <t>João</t>
-  </si>
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>Luiz</t>
-  </si>
-  <si>
-    <t>Alberto</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -82,39 +56,101 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -402,73 +438,90 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Idade</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>Nota</t>
+        </is>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3">
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="5" t="inlineStr">
+        <is>
+          <t>João</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="4" t="n">
         <v>5.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3">
-        <v>13</v>
-      </c>
-      <c r="C3" s="4">
-        <v>9.7</v>
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>9.699999999999999</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3">
+    <row r="4" ht="18.75" customHeight="1">
+      <c r="A4" s="5" t="inlineStr">
+        <is>
+          <t>Luiz</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="C4" s="4">
-        <v>8.8</v>
+      <c r="C4" s="4" t="n">
+        <v>8.800000000000001</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3">
+    <row r="5" ht="18.75" customHeight="1">
+      <c r="A5" s="5" t="inlineStr">
+        <is>
+          <t>Alberto</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="3" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>